<commit_message>
finish animations, update sprite inventory sheet
</commit_message>
<xml_diff>
--- a/assets/sprites_v1.xlsx
+++ b/assets/sprites_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rex\Documents\GitHub\octo-chainsaw\_assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rex\Documents\GitHub\octo-chainsaw\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -164,15 +164,9 @@
     <t>fx/swoosh-##</t>
   </si>
   <si>
-    <t>grid</t>
-  </si>
-  <si>
     <t>Targeting Arrow</t>
   </si>
   <si>
-    <t>hud/arrow</t>
-  </si>
-  <si>
     <t>hud/reticule</t>
   </si>
   <si>
@@ -267,6 +261,45 @@
   </si>
   <si>
     <t>H (px)</t>
+  </si>
+  <si>
+    <t>hud/targeting-arrow</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Start Screen</t>
+  </si>
+  <si>
+    <t>Play Over</t>
+  </si>
+  <si>
+    <t>Play Down</t>
+  </si>
+  <si>
+    <t>Play Up</t>
+  </si>
+  <si>
+    <t>Play Out</t>
+  </si>
+  <si>
+    <t>hud/grid</t>
+  </si>
+  <si>
+    <t>hud/logo</t>
+  </si>
+  <si>
+    <t>hud/play-over</t>
+  </si>
+  <si>
+    <t>hud/play-out</t>
+  </si>
+  <si>
+    <t>hud/play-down</t>
+  </si>
+  <si>
+    <t>hud/play-up</t>
   </si>
 </sst>
 </file>
@@ -607,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I44"/>
+  <dimension ref="B3:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>1</v>
@@ -638,10 +671,10 @@
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>28</v>
@@ -652,7 +685,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -678,7 +711,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -704,7 +737,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -756,7 +789,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -782,7 +815,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -803,12 +836,12 @@
         <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -829,12 +862,12 @@
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -855,12 +888,12 @@
         <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -881,12 +914,12 @@
         <v>29</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -907,12 +940,12 @@
         <v>29</v>
       </c>
       <c r="I14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -933,12 +966,12 @@
         <v>29</v>
       </c>
       <c r="I15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -959,12 +992,12 @@
         <v>29</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -985,7 +1018,7 @@
         <v>29</v>
       </c>
       <c r="I17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -1011,12 +1044,12 @@
         <v>29</v>
       </c>
       <c r="I18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1037,7 +1070,7 @@
         <v>29</v>
       </c>
       <c r="I19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -1045,7 +1078,7 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1071,7 +1104,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1097,7 +1130,7 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" s="1">
         <v>3</v>
@@ -1123,7 +1156,7 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D24" s="1">
         <v>3</v>
@@ -1149,7 +1182,7 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1175,7 +1208,7 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -1201,7 +1234,7 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
@@ -1227,7 +1260,7 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
@@ -1253,7 +1286,7 @@
         <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
@@ -1276,10 +1309,10 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
@@ -1297,47 +1330,59 @@
         <v>30</v>
       </c>
       <c r="I31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="1">
+        <v>4</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="1">
+        <v>24</v>
+      </c>
+      <c r="G33" s="1">
+        <v>24</v>
+      </c>
+      <c r="H33" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="1">
-        <v>4</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H33" t="s">
-        <v>54</v>
-      </c>
       <c r="I33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="1">
+        <v>4</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="1">
+        <v>24</v>
+      </c>
+      <c r="G34" s="1">
+        <v>24</v>
+      </c>
+      <c r="H34" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="1">
-        <v>4</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" t="s">
-        <v>54</v>
-      </c>
       <c r="I34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
@@ -1345,13 +1390,19 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D36" s="1">
         <v>6</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="F36" s="1">
+        <v>16</v>
+      </c>
+      <c r="G36" s="1">
+        <v>16</v>
       </c>
       <c r="H36" t="s">
         <v>30</v>
@@ -1365,13 +1416,19 @@
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D37" s="1">
         <v>3</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="F37" s="1">
+        <v>48</v>
+      </c>
+      <c r="G37" s="1">
+        <v>16</v>
       </c>
       <c r="H37" t="s">
         <v>30</v>
@@ -1385,13 +1442,19 @@
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="F38" s="1">
+        <v>8</v>
+      </c>
+      <c r="G38" s="1">
+        <v>16</v>
       </c>
       <c r="H38" t="s">
         <v>30</v>
@@ -1405,7 +1468,7 @@
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
@@ -1413,11 +1476,17 @@
       <c r="E40" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F40" s="1">
+        <v>150</v>
+      </c>
+      <c r="G40" s="1">
+        <v>150</v>
+      </c>
       <c r="H40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I40" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
@@ -1425,7 +1494,7 @@
         <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -1433,11 +1502,17 @@
       <c r="E41" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F41" s="1">
+        <v>36</v>
+      </c>
+      <c r="G41" s="1">
+        <v>5</v>
+      </c>
       <c r="H41" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -1445,7 +1520,7 @@
         <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1453,11 +1528,17 @@
       <c r="E42" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F42" s="1">
+        <v>26</v>
+      </c>
+      <c r="G42" s="1">
+        <v>3</v>
+      </c>
       <c r="H42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
@@ -1465,7 +1546,7 @@
         <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -1473,19 +1554,25 @@
       <c r="E43" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F43" s="1">
+        <v>24</v>
+      </c>
+      <c r="G43" s="1">
+        <v>24</v>
+      </c>
       <c r="H43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1493,11 +1580,147 @@
       <c r="E44" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F44" s="1">
+        <v>12</v>
+      </c>
+      <c r="G44" s="1">
+        <v>6</v>
+      </c>
       <c r="H44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I44" t="s">
-        <v>48</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="1">
+        <v>390</v>
+      </c>
+      <c r="G46" s="1">
+        <v>164</v>
+      </c>
+      <c r="H46" t="s">
+        <v>51</v>
+      </c>
+      <c r="I46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="1">
+        <v>168</v>
+      </c>
+      <c r="G47" s="1">
+        <v>72</v>
+      </c>
+      <c r="H47" t="s">
+        <v>51</v>
+      </c>
+      <c r="I47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F48" s="1">
+        <v>168</v>
+      </c>
+      <c r="G48" s="1">
+        <v>72</v>
+      </c>
+      <c r="H48" t="s">
+        <v>51</v>
+      </c>
+      <c r="I48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="1">
+        <v>168</v>
+      </c>
+      <c r="G49" s="1">
+        <v>72</v>
+      </c>
+      <c r="H49" t="s">
+        <v>51</v>
+      </c>
+      <c r="I49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" s="1">
+        <v>168</v>
+      </c>
+      <c r="G50" s="1">
+        <v>72</v>
+      </c>
+      <c r="H50" t="s">
+        <v>51</v>
+      </c>
+      <c r="I50" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update spritesheet reference table
</commit_message>
<xml_diff>
--- a/assets/sprites_v1.xlsx
+++ b/assets/sprites_v1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -101,9 +101,6 @@
     <t>player/move-##</t>
   </si>
   <si>
-    <t>player/fire-##</t>
-  </si>
-  <si>
     <t>player/hit-##</t>
   </si>
   <si>
@@ -191,18 +188,12 @@
     <t>enemy01/idle-##</t>
   </si>
   <si>
-    <t>enemy01/fire-##</t>
-  </si>
-  <si>
     <t>enemy01/die-##</t>
   </si>
   <si>
     <t>enemy02/move-##</t>
   </si>
   <si>
-    <t>enemy02/fire-##</t>
-  </si>
-  <si>
     <t>enemy02/die-##</t>
   </si>
   <si>
@@ -230,18 +221,12 @@
     <t>pickups/diamond-##</t>
   </si>
   <si>
-    <t>enemy03/fire-##</t>
-  </si>
-  <si>
     <t>Idle</t>
   </si>
   <si>
     <t>Move</t>
   </si>
   <si>
-    <t>Fire</t>
-  </si>
-  <si>
     <t>Die</t>
   </si>
   <si>
@@ -300,6 +285,27 @@
   </si>
   <si>
     <t>hud/play-up</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>player/attack-##</t>
+  </si>
+  <si>
+    <t>enemy02/attack-##</t>
+  </si>
+  <si>
+    <t>enemy03/attack-##</t>
+  </si>
+  <si>
+    <t>enemy01/move-##</t>
+  </si>
+  <si>
+    <t>Aim</t>
+  </si>
+  <si>
+    <t>enemy03/aim-##</t>
   </si>
 </sst>
 </file>
@@ -643,7 +649,7 @@
   <dimension ref="B3:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>1</v>
@@ -671,13 +677,13 @@
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>17</v>
@@ -685,7 +691,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -694,7 +700,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="1">
         <v>36</v>
@@ -703,7 +709,7 @@
         <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
@@ -711,7 +717,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -720,7 +726,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1">
         <v>36</v>
@@ -729,7 +735,7 @@
         <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
@@ -737,7 +743,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -746,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1">
         <v>36</v>
@@ -755,15 +761,15 @@
         <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -772,7 +778,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1">
         <v>36</v>
@@ -781,15 +787,15 @@
         <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -798,7 +804,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1">
         <v>36</v>
@@ -807,15 +813,15 @@
         <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -824,7 +830,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1">
         <v>24</v>
@@ -833,15 +839,15 @@
         <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -850,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1">
         <v>24</v>
@@ -859,15 +865,15 @@
         <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -876,7 +882,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="1">
         <v>24</v>
@@ -885,15 +891,15 @@
         <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -902,7 +908,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="1">
         <v>36</v>
@@ -911,15 +917,15 @@
         <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -928,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1">
         <v>36</v>
@@ -937,15 +943,15 @@
         <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -954,7 +960,7 @@
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1">
         <v>36</v>
@@ -963,15 +969,15 @@
         <v>36</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -980,24 +986,24 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G16" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -1006,24 +1012,24 @@
         <v>4</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G17" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I17" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -1032,24 +1038,24 @@
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G18" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1058,19 +1064,19 @@
         <v>4</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G19" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -1078,13 +1084,13 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" s="1">
         <v>17</v>
@@ -1093,10 +1099,10 @@
         <v>40</v>
       </c>
       <c r="H21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" t="s">
         <v>30</v>
-      </c>
-      <c r="I21" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -1104,13 +1110,13 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="1">
         <v>17</v>
@@ -1119,10 +1125,10 @@
         <v>40</v>
       </c>
       <c r="H22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -1130,13 +1136,13 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D23" s="1">
         <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="1">
         <v>48</v>
@@ -1145,10 +1151,10 @@
         <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1156,13 +1162,13 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D24" s="1">
         <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="1">
         <v>8</v>
@@ -1171,10 +1177,10 @@
         <v>24</v>
       </c>
       <c r="H24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -1182,13 +1188,13 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="1">
         <v>5</v>
@@ -1197,10 +1203,10 @@
         <v>24</v>
       </c>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -1208,13 +1214,13 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F26" s="1">
         <v>16</v>
@@ -1223,10 +1229,10 @@
         <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -1234,13 +1240,13 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="1">
         <v>20</v>
@@ -1249,10 +1255,10 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -1260,13 +1266,13 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="1">
         <v>20</v>
@@ -1275,10 +1281,10 @@
         <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -1286,13 +1292,13 @@
         <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" s="1">
         <v>20</v>
@@ -1301,24 +1307,24 @@
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="1">
         <v>48</v>
@@ -1327,24 +1333,24 @@
         <v>32</v>
       </c>
       <c r="H31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1">
         <v>4</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33" s="1">
         <v>24</v>
@@ -1353,24 +1359,24 @@
         <v>24</v>
       </c>
       <c r="H33" t="s">
+        <v>51</v>
+      </c>
+      <c r="I33" t="s">
         <v>52</v>
-      </c>
-      <c r="I33" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D34" s="1">
         <v>4</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F34" s="1">
         <v>24</v>
@@ -1379,24 +1385,24 @@
         <v>24</v>
       </c>
       <c r="H34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D36" s="1">
         <v>6</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F36" s="1">
         <v>16</v>
@@ -1405,10 +1411,10 @@
         <v>16</v>
       </c>
       <c r="H36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
@@ -1416,13 +1422,13 @@
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D37" s="1">
         <v>3</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F37" s="1">
         <v>48</v>
@@ -1431,10 +1437,10 @@
         <v>16</v>
       </c>
       <c r="H37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
@@ -1442,13 +1448,13 @@
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F38" s="1">
         <v>8</v>
@@ -1457,10 +1463,10 @@
         <v>16</v>
       </c>
       <c r="H38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
@@ -1468,13 +1474,13 @@
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F40" s="1">
         <v>150</v>
@@ -1483,10 +1489,10 @@
         <v>150</v>
       </c>
       <c r="H40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I40" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
@@ -1494,13 +1500,13 @@
         <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F41" s="1">
         <v>36</v>
@@ -1509,10 +1515,10 @@
         <v>5</v>
       </c>
       <c r="H41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -1520,13 +1526,13 @@
         <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F42" s="1">
         <v>26</v>
@@ -1535,10 +1541,10 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
@@ -1546,13 +1552,13 @@
         <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F43" s="1">
         <v>24</v>
@@ -1561,24 +1567,24 @@
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F44" s="1">
         <v>12</v>
@@ -1587,24 +1593,24 @@
         <v>6</v>
       </c>
       <c r="H44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I44" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F46" s="1">
         <v>390</v>
@@ -1613,24 +1619,24 @@
         <v>164</v>
       </c>
       <c r="H46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I46" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F47" s="1">
         <v>168</v>
@@ -1639,24 +1645,24 @@
         <v>72</v>
       </c>
       <c r="H47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I47" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F48" s="1">
         <v>168</v>
@@ -1665,24 +1671,24 @@
         <v>72</v>
       </c>
       <c r="H48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I48" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F49" s="1">
         <v>168</v>
@@ -1691,24 +1697,24 @@
         <v>72</v>
       </c>
       <c r="H49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I49" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F50" s="1">
         <v>168</v>
@@ -1717,10 +1723,10 @@
         <v>72</v>
       </c>
       <c r="H50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I50" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update game assets and sprites spreadsheet
</commit_message>
<xml_diff>
--- a/assets/sprites_v1.xlsx
+++ b/assets/sprites_v1.xlsx
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,10 +1093,10 @@
         <v>40</v>
       </c>
       <c r="F21" s="1">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="G21" s="1">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
         <v>29</v>
@@ -1119,10 +1119,10 @@
         <v>40</v>
       </c>
       <c r="F22" s="1">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="G22" s="1">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="H22" t="s">
         <v>29</v>

</xml_diff>